<commit_message>
26: changed admin_confirmed column in CandidateConfirmation to verified.
</commit_message>
<xml_diff>
--- a/spec/fixtures/export_with_events.xlsx
+++ b/spec/fixtures/export_with_events.xlsx
@@ -68,13 +68,13 @@
     <t>candidate_events.0.completed_date</t>
   </si>
   <si>
-    <t>candidate_events.0.admin_confirmed</t>
+    <t>candidate_events.0.verified</t>
   </si>
   <si>
     <t>candidate_events.1.completed_date</t>
   </si>
   <si>
-    <t>candidate_events.1.admin_confirmed</t>
+    <t>candidate_events.1.verified</t>
   </si>
   <si>
     <t>vickikristoff</t>

</xml_diff>

<commit_message>
27: added column instructions to confirmation_events
</commit_message>
<xml_diff>
--- a/spec/fixtures/export_with_events.xlsx
+++ b/spec/fixtures/export_with_events.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>name</t>
   </si>
@@ -20,10 +20,25 @@
     <t>due_date</t>
   </si>
   <si>
+    <t>instructions</t>
+  </si>
+  <si>
+    <t>Attend Retreat</t>
+  </si>
+  <si>
+    <t>&lt;h1&gt;a heading&lt;/h1&gt;
+&lt;ul&gt;
+&lt;li&gt;step 1&lt;/li&gt;
+&lt;li&gt;step 2&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt; &lt;/p&gt;
+&lt;p&gt; &lt;/p&gt;</t>
+  </si>
+  <si>
     <t>Parent Information Meeting</t>
   </si>
   <si>
-    <t>Attend Retreat</t>
+    <t>&lt;p&gt;&lt;em&gt;&lt;strong&gt;simple text&lt;/strong&gt;&lt;/em&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>account_name</t>
@@ -207,7 +222,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -217,13 +232,19 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -385,7 +406,13 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -484,10 +511,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica"/>
+            <a:latin typeface="Cambria"/>
+            <a:ea typeface="Cambria"/>
+            <a:cs typeface="Cambria"/>
+            <a:sym typeface="Cambria"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -742,7 +769,13 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1055,10 +1088,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica"/>
+            <a:latin typeface="Cambria"/>
+            <a:ea typeface="Cambria"/>
+            <a:cs typeface="Cambria"/>
+            <a:sym typeface="Cambria"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1317,7 +1350,7 @@
   <cols>
     <col min="1" max="1" width="19.8516" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.1719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="1" customWidth="1"/>
+    <col min="3" max="3" width="78.1719" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.85156" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.85156" style="1" customWidth="1"/>
     <col min="6" max="256" width="8.85156" style="1" customWidth="1"/>
@@ -1330,29 +1363,35 @@
       <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" ht="14.6" customHeight="1">
+    <row r="2" ht="86.6" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4">
-        <v>42524</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>42493</v>
+      </c>
+      <c r="C2" t="s" s="5">
+        <v>4</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" ht="14.6" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4">
-        <v>42493</v>
-      </c>
-      <c r="C3" s="3"/>
+        <v>42524</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>6</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
@@ -1422,215 +1461,215 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11" style="5" customWidth="1"/>
-    <col min="2" max="2" width="7.67188" style="5" customWidth="1"/>
-    <col min="3" max="3" width="7.67188" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.1719" style="5" customWidth="1"/>
-    <col min="6" max="6" width="12.1719" style="5" customWidth="1"/>
-    <col min="7" max="7" width="6.67188" style="5" customWidth="1"/>
-    <col min="8" max="8" width="16.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="17.6719" style="5" customWidth="1"/>
-    <col min="10" max="10" width="11" style="5" customWidth="1"/>
-    <col min="11" max="11" width="7.67188" style="5" customWidth="1"/>
-    <col min="12" max="12" width="7.67188" style="5" customWidth="1"/>
-    <col min="13" max="13" width="12.1719" style="5" customWidth="1"/>
-    <col min="14" max="14" width="24.1719" style="5" customWidth="1"/>
-    <col min="15" max="15" width="24.1719" style="5" customWidth="1"/>
-    <col min="16" max="16" width="24.1719" style="5" customWidth="1"/>
-    <col min="17" max="17" width="24.1719" style="5" customWidth="1"/>
-    <col min="18" max="256" width="8.85156" style="5" customWidth="1"/>
+    <col min="1" max="1" width="11" style="6" customWidth="1"/>
+    <col min="2" max="2" width="7.67188" style="6" customWidth="1"/>
+    <col min="3" max="3" width="7.67188" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11" style="6" customWidth="1"/>
+    <col min="5" max="5" width="12.1719" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.1719" style="6" customWidth="1"/>
+    <col min="7" max="7" width="6.67188" style="6" customWidth="1"/>
+    <col min="8" max="8" width="16.5" style="6" customWidth="1"/>
+    <col min="9" max="9" width="14.3516" style="6" customWidth="1"/>
+    <col min="10" max="10" width="11" style="6" customWidth="1"/>
+    <col min="11" max="11" width="7.67188" style="6" customWidth="1"/>
+    <col min="12" max="12" width="7.67188" style="6" customWidth="1"/>
+    <col min="13" max="13" width="12.1719" style="6" customWidth="1"/>
+    <col min="14" max="14" width="24.1719" style="6" customWidth="1"/>
+    <col min="15" max="15" width="18.6719" style="6" customWidth="1"/>
+    <col min="16" max="16" width="24.1719" style="6" customWidth="1"/>
+    <col min="17" max="17" width="18.6719" style="6" customWidth="1"/>
+    <col min="18" max="256" width="8.85156" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K1" t="s" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L1" t="s" s="2">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M1" t="s" s="2">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N1" t="s" s="2">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="O1" t="s" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="P1" t="s" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="Q1" t="s" s="2">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="14.6" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="G2" s="3">
+        <v>28</v>
+      </c>
+      <c r="G2" s="7">
         <v>12</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s" s="2">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="M2" s="3">
+        <v>32</v>
+      </c>
+      <c r="M2" s="7">
         <v>27502</v>
       </c>
       <c r="N2" s="4">
         <v>42527</v>
       </c>
-      <c r="O2" t="b" s="6">
+      <c r="O2" t="b" s="8">
         <v>1</v>
       </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" t="b" s="6">
+      <c r="P2" s="7"/>
+      <c r="Q2" t="b" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="3" ht="14.6" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="G3" s="3">
+        <v>27</v>
+      </c>
+      <c r="G3" s="7">
         <v>9</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s" s="2">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="M3" s="3">
+        <v>32</v>
+      </c>
+      <c r="M3" s="7">
         <v>27555</v>
       </c>
-      <c r="N3" s="3"/>
-      <c r="O3" t="b" s="6">
+      <c r="N3" s="7"/>
+      <c r="O3" t="b" s="8">
         <v>0</v>
       </c>
       <c r="P3" s="4">
         <v>42492</v>
       </c>
-      <c r="Q3" t="b" s="6">
+      <c r="Q3" t="b" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="4" ht="14.6" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="3">
+      <c r="G4" s="7">
         <v>10</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" t="s" s="2">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="M4" s="3">
+        <v>44</v>
+      </c>
+      <c r="M4" s="7">
         <v>47129</v>
       </c>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
     </row>
     <row r="5" ht="14.6" customHeight="1">
       <c r="A5" s="3"/>

</xml_diff>

<commit_message>
22: temp commit: sign agreement
</commit_message>
<xml_diff>
--- a/spec/fixtures/export_with_events.xlsx
+++ b/spec/fixtures/export_with_events.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>name</t>
   </si>
@@ -26,6 +26,9 @@
     <t>Attend Retreat</t>
   </si>
   <si>
+    <t>Sign Agreement</t>
+  </si>
+  <si>
     <t>account_name</t>
   </si>
   <si>
@@ -75,6 +78,12 @@
   </si>
   <si>
     <t>candidate_events.1.admin_confirmed</t>
+  </si>
+  <si>
+    <t>candidate_events.2.completed_date</t>
+  </si>
+  <si>
+    <t>candidate_events.2.admin_confirmed</t>
   </si>
   <si>
     <t>vickikristoff</t>
@@ -147,7 +156,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -162,6 +171,11 @@
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="11"/>
+      <name val="Menlo"/>
     </font>
   </fonts>
   <fills count="3">
@@ -207,7 +221,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -221,6 +235,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -248,6 +265,7 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff040303"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1315,7 +1333,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1719" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.1719" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.85156" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.85156" style="1" customWidth="1"/>
@@ -1357,8 +1375,12 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" ht="14.6" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" t="s" s="5">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>42564</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1416,119 +1438,129 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11" style="5" customWidth="1"/>
-    <col min="2" max="2" width="7.67188" style="5" customWidth="1"/>
-    <col min="3" max="3" width="7.67188" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.1719" style="5" customWidth="1"/>
-    <col min="6" max="6" width="12.1719" style="5" customWidth="1"/>
-    <col min="7" max="7" width="6.67188" style="5" customWidth="1"/>
-    <col min="8" max="8" width="16.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="17.6719" style="5" customWidth="1"/>
-    <col min="10" max="10" width="11" style="5" customWidth="1"/>
-    <col min="11" max="11" width="7.67188" style="5" customWidth="1"/>
-    <col min="12" max="12" width="7.67188" style="5" customWidth="1"/>
-    <col min="13" max="13" width="12.1719" style="5" customWidth="1"/>
-    <col min="14" max="14" width="24.1719" style="5" customWidth="1"/>
-    <col min="15" max="15" width="24.1719" style="5" customWidth="1"/>
-    <col min="16" max="16" width="24.1719" style="5" customWidth="1"/>
-    <col min="17" max="17" width="24.1719" style="5" customWidth="1"/>
-    <col min="18" max="256" width="8.85156" style="5" customWidth="1"/>
+    <col min="1" max="1" width="11" style="6" customWidth="1"/>
+    <col min="2" max="2" width="7.67188" style="6" customWidth="1"/>
+    <col min="3" max="3" width="7.67188" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11" style="6" customWidth="1"/>
+    <col min="5" max="5" width="12.1719" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.1719" style="6" customWidth="1"/>
+    <col min="7" max="7" width="6.67188" style="6" customWidth="1"/>
+    <col min="8" max="8" width="16.5" style="6" customWidth="1"/>
+    <col min="9" max="9" width="17.6719" style="6" customWidth="1"/>
+    <col min="10" max="10" width="11" style="6" customWidth="1"/>
+    <col min="11" max="11" width="7.67188" style="6" customWidth="1"/>
+    <col min="12" max="12" width="7.67188" style="6" customWidth="1"/>
+    <col min="13" max="13" width="12.1719" style="6" customWidth="1"/>
+    <col min="14" max="14" width="24.1719" style="6" customWidth="1"/>
+    <col min="15" max="15" width="24.1719" style="6" customWidth="1"/>
+    <col min="16" max="16" width="24.1719" style="6" customWidth="1"/>
+    <col min="17" max="17" width="24.1719" style="6" customWidth="1"/>
+    <col min="18" max="18" width="24.1719" style="6" customWidth="1"/>
+    <col min="19" max="19" width="24.1719" style="6" customWidth="1"/>
+    <col min="20" max="20" width="24.1719" style="6" customWidth="1"/>
+    <col min="21" max="256" width="8.85156" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K1" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L1" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M1" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N1" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O1" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P1" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q1" t="s" s="2">
-        <v>20</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="R1" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="T1" s="2"/>
     </row>
     <row r="2" ht="14.6" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G2" s="3">
         <v>12</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s" s="2">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M2" s="3">
         <v>27502</v>
@@ -1536,93 +1568,103 @@
       <c r="N2" s="4">
         <v>42527</v>
       </c>
-      <c r="O2" t="b" s="6">
+      <c r="O2" t="b" s="7">
         <v>1</v>
       </c>
       <c r="P2" s="3"/>
-      <c r="Q2" t="b" s="6">
+      <c r="Q2" t="b" s="7">
         <v>0</v>
       </c>
+      <c r="R2" s="4">
+        <v>42441</v>
+      </c>
+      <c r="S2" t="b" s="7">
+        <v>1</v>
+      </c>
+      <c r="T2" s="3"/>
     </row>
     <row r="3" ht="14.6" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G3" s="3">
         <v>9</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s" s="2">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M3" s="3">
         <v>27555</v>
       </c>
       <c r="N3" s="3"/>
-      <c r="O3" t="b" s="6">
+      <c r="O3" t="b" s="7">
         <v>0</v>
       </c>
       <c r="P3" s="4">
         <v>42492</v>
       </c>
-      <c r="Q3" t="b" s="6">
+      <c r="Q3" t="b" s="7">
         <v>1</v>
       </c>
+      <c r="R3" s="4"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
     </row>
     <row r="4" ht="14.6" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3">
         <v>10</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" t="s" s="2">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="M4" s="3">
         <v>47129</v>
@@ -1631,6 +1673,9 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
     </row>
     <row r="5" ht="14.6" customHeight="1">
       <c r="A5" s="3"/>
@@ -1650,6 +1695,9 @@
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
     </row>
     <row r="6" ht="14.6" customHeight="1">
       <c r="A6" s="3"/>
@@ -1669,6 +1717,9 @@
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
     </row>
     <row r="7" ht="14.6" customHeight="1">
       <c r="A7" s="3"/>
@@ -1688,6 +1739,9 @@
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
     </row>
     <row r="8" ht="14.6" customHeight="1">
       <c r="A8" s="3"/>
@@ -1707,6 +1761,9 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
     </row>
     <row r="9" ht="14.6" customHeight="1">
       <c r="A9" s="3"/>
@@ -1726,6 +1783,9 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
     </row>
     <row r="10" ht="14.6" customHeight="1">
       <c r="A10" s="3"/>
@@ -1745,6 +1805,9 @@
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
15: aded Candidate Sheet + ordered events: import was broken
</commit_message>
<xml_diff>
--- a/spec/fixtures/export_with_events.xlsx
+++ b/spec/fixtures/export_with_events.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>name</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Parent Information Meeting</t>
+  </si>
+  <si>
+    <t>Fill Out Candidate Information Sheet</t>
   </si>
   <si>
     <t>account_name</t>
@@ -1403,9 +1406,15 @@
       <c r="E4" s="3"/>
     </row>
     <row r="5" ht="14.6" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="A5" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>42416</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>4</v>
+      </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
@@ -1492,97 +1501,97 @@
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L1" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M1" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N1" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O1" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P1" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q1" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R1" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S1" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" ht="14.6" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G2" s="3">
         <v>12</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M2" s="3">
         <v>27502</v>
@@ -1604,38 +1613,38 @@
     </row>
     <row r="3" ht="14.6" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="E3" t="s" s="2">
-        <v>30</v>
-      </c>
       <c r="F3" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G3" s="3">
         <v>9</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M3" s="3">
         <v>27555</v>
@@ -1659,34 +1668,34 @@
     </row>
     <row r="4" ht="14.6" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3">
         <v>10</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M4" s="3">
         <v>47129</v>

</xml_diff>

<commit_message>
16: added baptismal certificate uploading and adding the appropriate data.
</commit_message>
<xml_diff>
--- a/spec/fixtures/export_with_events.xlsx
+++ b/spec/fixtures/export_with_events.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>name</t>
   </si>
@@ -47,6 +47,12 @@
     <t>Fill Out Candidate Information Sheet</t>
   </si>
   <si>
+    <t>Upload Baptismal Certificate</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;&lt;strong&gt;Upload certificate&lt;/strong&gt;&lt;/em&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>account_name</t>
   </si>
   <si>
@@ -102,6 +108,18 @@
   </si>
   <si>
     <t>candidate_events.2.verified</t>
+  </si>
+  <si>
+    <t>candidate_events.3.completed_date</t>
+  </si>
+  <si>
+    <t>candidate_events.3.verified</t>
+  </si>
+  <si>
+    <t>candidate_events.4.completed_date</t>
+  </si>
+  <si>
+    <t>candidate_events.4.verified</t>
   </si>
   <si>
     <t>vickikristoff</t>
@@ -1345,7 +1363,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33.7969" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.1719" style="1" customWidth="1"/>
     <col min="3" max="3" width="78.1719" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.85156" style="1" customWidth="1"/>
@@ -1419,9 +1437,15 @@
       <c r="E5" s="3"/>
     </row>
     <row r="6" ht="14.6" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="A6" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>42594</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>10</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
@@ -1471,7 +1495,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1496,102 +1520,118 @@
     <col min="17" max="17" width="18.6719" style="6" customWidth="1"/>
     <col min="18" max="18" width="18.6719" style="6" customWidth="1"/>
     <col min="19" max="19" width="18.6719" style="6" customWidth="1"/>
-    <col min="20" max="256" width="8.85156" style="6" customWidth="1"/>
+    <col min="20" max="20" width="18.6719" style="6" customWidth="1"/>
+    <col min="21" max="21" width="18.6719" style="6" customWidth="1"/>
+    <col min="22" max="22" width="18.6719" style="6" customWidth="1"/>
+    <col min="23" max="23" width="18.6719" style="6" customWidth="1"/>
+    <col min="24" max="256" width="8.85156" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K1" t="s" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L1" t="s" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M1" t="s" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N1" t="s" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O1" t="s" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Q1" t="s" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="R1" t="s" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="S1" t="s" s="2">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="T1" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="U1" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="V1" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="W1" t="s" s="2">
+        <v>33</v>
       </c>
     </row>
     <row r="2" ht="14.6" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G2" s="3">
         <v>12</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s" s="2">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="M2" s="3">
         <v>27502</v>
@@ -1610,41 +1650,49 @@
       <c r="S2" t="b" s="7">
         <v>0</v>
       </c>
+      <c r="T2" s="3"/>
+      <c r="U2" t="b" s="7">
+        <v>0</v>
+      </c>
+      <c r="V2" s="3"/>
+      <c r="W2" t="b" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" ht="14.6" customHeight="1">
       <c r="A3" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="B3" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>31</v>
-      </c>
       <c r="F3" t="s" s="2">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G3" s="3">
         <v>9</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="M3" s="3">
         <v>27555</v>
@@ -1665,37 +1713,45 @@
       <c r="S3" t="b" s="7">
         <v>0</v>
       </c>
+      <c r="T3" s="4"/>
+      <c r="U3" t="b" s="7">
+        <v>0</v>
+      </c>
+      <c r="V3" s="4"/>
+      <c r="W3" t="b" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" ht="14.6" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3">
         <v>10</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" t="s" s="2">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="M4" s="3">
         <v>47129</v>
@@ -1706,6 +1762,10 @@
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
     </row>
     <row r="5" ht="14.6" customHeight="1">
       <c r="A5" s="3"/>
@@ -1727,6 +1787,10 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
     </row>
     <row r="6" ht="14.6" customHeight="1">
       <c r="A6" s="3"/>
@@ -1748,6 +1812,10 @@
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
     </row>
     <row r="7" ht="14.6" customHeight="1">
       <c r="A7" s="3"/>
@@ -1769,6 +1837,10 @@
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
     </row>
     <row r="8" ht="14.6" customHeight="1">
       <c r="A8" s="3"/>
@@ -1790,6 +1862,10 @@
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
     </row>
     <row r="9" ht="14.6" customHeight="1">
       <c r="A9" s="3"/>
@@ -1811,6 +1887,10 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
     </row>
     <row r="10" ht="14.6" customHeight="1">
       <c r="A10" s="3"/>
@@ -1832,6 +1912,10 @@
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>